<commit_message>
Tabellen und Excel etabliert.
</commit_message>
<xml_diff>
--- a/Test_Excel.xlsx
+++ b/Test_Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekte\table-data-processor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72AACB9-964F-41CC-90B9-B268EEA99B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916EB3B8-3943-4C22-848F-CC79074DE4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -517,7 +517,7 @@
         <v>35796</v>
       </c>
       <c r="H5" s="1">
-        <v>39938</v>
+        <v>46022</v>
       </c>
     </row>
   </sheetData>

</xml_diff>